<commit_message>
Minor changes to plots and notebooks
</commit_message>
<xml_diff>
--- a/data/raw_data/Material_content.xlsx
+++ b/data/raw_data/Material_content.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Box/BATMAN/Coding/V2G_in_EU/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A57EDB-9067-7143-B06B-16DEBEAF104D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5170FB7-07D8-1B42-83B9-E08036CD565A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35060" yWindow="500" windowWidth="33740" windowHeight="28300" activeTab="8" xr2:uid="{730E730F-0C19-714B-9567-4CAB8EE7D98A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{730E730F-0C19-714B-9567-4CAB8EE7D98A}"/>
   </bookViews>
   <sheets>
     <sheet name="kg per pack" sheetId="1" r:id="rId1"/>
@@ -247,8 +247,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -331,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -359,6 +360,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,7 +678,7 @@
   <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:P55"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6773,15 +6775,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC94FBC5-566A-0842-9AC8-CAC13902549B}">
-  <dimension ref="A1:N79"/>
+  <dimension ref="A1:R79"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -6819,7 +6821,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -6863,7 +6865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>38</v>
       </c>
@@ -6915,8 +6917,9 @@
         <f t="shared" si="0"/>
         <v>7.9330609585507936</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R3" s="11"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -6957,7 +6960,7 @@
         <v>3.3735275837026633</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -6998,7 +7001,7 @@
         <v>4.5595333748481304</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>14</v>
       </c>
@@ -7039,7 +7042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -7080,7 +7083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>16</v>
       </c>
@@ -7121,7 +7124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -7162,7 +7165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>29</v>
       </c>
@@ -7203,7 +7206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>30</v>
       </c>
@@ -7244,7 +7247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>31</v>
       </c>
@@ -7285,7 +7288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>32</v>
       </c>
@@ -7326,7 +7329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -7367,7 +7370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -7411,7 +7414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>38</v>
       </c>
@@ -19428,8 +19431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{519D7ED6-2302-9845-8693-BD9CC80CE476}">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>